<commit_message>
final model with video
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academics\Udacity\SDCE\CVSF\CarND_P4_BehaviorCloning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D73053AB-CBD1-45C8-BE55-C1A5EA2D6B0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCAA1E8-3510-483D-B85E-DAEB16B61782}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ABCAD1B5-EC46-4200-919B-E2E90178A3A5}"/>
   </bookViews>
@@ -196,24 +196,18 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>Sheet1!$A$2:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>9.4500000000000001E-2</c:v>
+                  <c:v>2.5499999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.5899999999999995E-2</c:v>
+                  <c:v>2.1299999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0999999999999994E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.7699999999999996E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.59E-2</c:v>
+                  <c:v>1.9699999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -253,24 +247,18 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:f>Sheet1!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.10730000000000001</c:v>
+                  <c:v>2.1499999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.8400000000000001E-2</c:v>
+                  <c:v>2.0299999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1008</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.4500000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.1300000000000006E-2</c:v>
+                  <c:v>1.9E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1487,10 +1475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64AD348B-026E-42AE-A07F-E2CE7522877E}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,42 +1497,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>9.4500000000000001E-2</v>
+        <v>2.5499999999999998E-2</v>
       </c>
       <c r="B2">
-        <v>0.10730000000000001</v>
+        <v>2.1499999999999998E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>7.5899999999999995E-2</v>
+        <v>2.1299999999999999E-2</v>
       </c>
       <c r="B3">
-        <v>9.8400000000000001E-2</v>
+        <v>2.0299999999999999E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>7.0999999999999994E-2</v>
+        <v>1.9699999999999999E-2</v>
       </c>
       <c r="B4">
-        <v>0.1008</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>6.7699999999999996E-2</v>
-      </c>
-      <c r="B5">
-        <v>9.4500000000000001E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6.59E-2</v>
-      </c>
-      <c r="B6">
-        <v>9.1300000000000006E-2</v>
+        <v>1.9E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>